<commit_message>
Added ways for CSV, TSV, and possibly Excel to be worked with, as well as a more streamlined way of recognizing and adapting to the different file types.
</commit_message>
<xml_diff>
--- a/Programs/dependencies_test/GFGsheet.xlsx
+++ b/Programs/dependencies_test/GFGsheet.xlsx
@@ -6,13 +6,15 @@
     <workbookView activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Research Data; RePORTER_PRJ_X_F" r:id="rId3" sheetId="1"/>
+    <sheet name="RePORTER_PRJ_X_FY2022_002.xml" r:id="rId3" sheetId="1"/>
+    <sheet name="RePORTER_PRJ_C_FY2021_053.csv" r:id="rId4" sheetId="2"/>
+    <sheet name="SearchResults.tsv" r:id="rId5" sheetId="3"/>
   </sheets>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="140">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="339" uniqueCount="284">
   <si>
     <t>APPLICATION_ID</t>
   </si>
@@ -433,6 +435,438 @@
   </si>
   <si>
     <t>DAVIS, BRETT  (contact)</t>
+  </si>
+  <si>
+    <t>PI_NAMEs</t>
+  </si>
+  <si>
+    <t>10492112</t>
+  </si>
+  <si>
+    <t>SCHER, HOWARD I;</t>
+  </si>
+  <si>
+    <t>10491389</t>
+  </si>
+  <si>
+    <t>ALBUQUERQUE</t>
+  </si>
+  <si>
+    <t>WILLMAN, CHERYL L.;</t>
+  </si>
+  <si>
+    <t>10469107</t>
+  </si>
+  <si>
+    <t>KANSAS CITY</t>
+  </si>
+  <si>
+    <t>PIOTROWSKI, TATJANA ;</t>
+  </si>
+  <si>
+    <t>10435766</t>
+  </si>
+  <si>
+    <t>TEMPE</t>
+  </si>
+  <si>
+    <t>LEE, HYUNGLAE ;</t>
+  </si>
+  <si>
+    <t>10430592</t>
+  </si>
+  <si>
+    <t>RALEIGH</t>
+  </si>
+  <si>
+    <t>LESTER, JAMES CURTIS;</t>
+  </si>
+  <si>
+    <t>10415597</t>
+  </si>
+  <si>
+    <t>GLIMCHER, LAURIE HOLLIS;</t>
+  </si>
+  <si>
+    <t>10406624</t>
+  </si>
+  <si>
+    <t>HENDERSHOT, CHRISTIAN S;</t>
+  </si>
+  <si>
+    <t>10401518</t>
+  </si>
+  <si>
+    <t>NOWAK, REBECCA G.;</t>
+  </si>
+  <si>
+    <t>10391927</t>
+  </si>
+  <si>
+    <t>GURABO</t>
+  </si>
+  <si>
+    <t>CUNCI, LISANDRO FEDERICO (contact); DOBRUNZ, LYNN E;</t>
+  </si>
+  <si>
+    <t>10374223</t>
+  </si>
+  <si>
+    <t>GARCIA-MARTINEZ, J. VICTOR ; SARTOR, RYAN B; WAHL, ANGELA RAQUEL (contact);</t>
+  </si>
+  <si>
+    <t>10373516</t>
+  </si>
+  <si>
+    <t>MOSQUERA-LOPEZ, CLARA MARCELA;</t>
+  </si>
+  <si>
+    <t>10370926</t>
+  </si>
+  <si>
+    <t>JENSEN, BRYAN C;</t>
+  </si>
+  <si>
+    <t>10366502</t>
+  </si>
+  <si>
+    <t>VAN DER HOEVEN, RANSOME ;</t>
+  </si>
+  <si>
+    <t>10364898</t>
+  </si>
+  <si>
+    <t>CHEN, ZHIYUAN ;</t>
+  </si>
+  <si>
+    <t>10364135</t>
+  </si>
+  <si>
+    <t>NASHVILLE</t>
+  </si>
+  <si>
+    <t>REYNOLDS, WILLIAM STUART;</t>
+  </si>
+  <si>
+    <t>10363984</t>
+  </si>
+  <si>
+    <t>LAFERRERE, BLANDINE B; ST-ONGE, MARIE-PIERRE  (contact);</t>
+  </si>
+  <si>
+    <t>10353171</t>
+  </si>
+  <si>
+    <t>CORNACCHIONE (ROSS), JENNIFER JANE; RANNEY, LEAH MARIE (contact);</t>
+  </si>
+  <si>
+    <t>10351373</t>
+  </si>
+  <si>
+    <t>SCALEA, JOSEPH R.;</t>
+  </si>
+  <si>
+    <t>10343091</t>
+  </si>
+  <si>
+    <t>SAINT LOUIS</t>
+  </si>
+  <si>
+    <t>JAIN, AJAY K.;</t>
+  </si>
+  <si>
+    <t>10328118</t>
+  </si>
+  <si>
+    <t>VILLANI, ALEXANDRA-CHLOE ;</t>
+  </si>
+  <si>
+    <t>10327842</t>
+  </si>
+  <si>
+    <t>MILLER, OSCAR ;</t>
+  </si>
+  <si>
+    <t>10327839</t>
+  </si>
+  <si>
+    <t>MU, RICHARD ;</t>
+  </si>
+  <si>
+    <t>10320332</t>
+  </si>
+  <si>
+    <t>BUTTS, JESSICA CHRISTINE;</t>
+  </si>
+  <si>
+    <t>10303458</t>
+  </si>
+  <si>
+    <t>PEOPLES, ROBERT WILLIAM;</t>
+  </si>
+  <si>
+    <t>10302840</t>
+  </si>
+  <si>
+    <t>BENN, EMMA KATHERINE TARA;</t>
+  </si>
+  <si>
+    <t>10302548</t>
+  </si>
+  <si>
+    <t>SPERBER, NINA ;</t>
+  </si>
+  <si>
+    <t>10298680</t>
+  </si>
+  <si>
+    <t>BINGHAMTON</t>
+  </si>
+  <si>
+    <t>WAN, YUAN ;</t>
+  </si>
+  <si>
+    <t>10298453</t>
+  </si>
+  <si>
+    <t>SALT LAKE CITY</t>
+  </si>
+  <si>
+    <t>RAMKUMAR, NIRUPAMA ;</t>
+  </si>
+  <si>
+    <t>10295401</t>
+  </si>
+  <si>
+    <t>LEDER, BENJAMIN Z;</t>
+  </si>
+  <si>
+    <t>10294888</t>
+  </si>
+  <si>
+    <t>Los Angeles</t>
+  </si>
+  <si>
+    <t>BAEZCONDE-GARBANATI, LOURDES A.;</t>
+  </si>
+  <si>
+    <t>10294462</t>
+  </si>
+  <si>
+    <t>NEW HAVEN</t>
+  </si>
+  <si>
+    <t>CLAUS, ELIZABETH B. (contact); KWAN, BETHANY MATTHEWS; VERHAAK, ROEL GW;</t>
+  </si>
+  <si>
+    <t>10292752</t>
+  </si>
+  <si>
+    <t>OKLAHOMA CITY</t>
+  </si>
+  <si>
+    <t>MANNEL, ROBERT S;</t>
+  </si>
+  <si>
+    <t>10290163</t>
+  </si>
+  <si>
+    <t>RICHMOND</t>
+  </si>
+  <si>
+    <t>CLEVENGER, CHARLES V;</t>
+  </si>
+  <si>
+    <t>10290159</t>
+  </si>
+  <si>
+    <t>HUGHES-HALBERT, CHANITA A; SEEWALDT, VICTORIA L.; WINN, ROBERT A. (contact);</t>
+  </si>
+  <si>
+    <t>10279165</t>
+  </si>
+  <si>
+    <t>CAMBRIDGE</t>
+  </si>
+  <si>
+    <t>ABUDAYYEH, OMAR O (contact); GOOTENBERG, JONATHAN SAMUEL;</t>
+  </si>
+  <si>
+    <t>10276515</t>
+  </si>
+  <si>
+    <t>GARZA, LUIS ANDRES;</t>
+  </si>
+  <si>
+    <t>10274928</t>
+  </si>
+  <si>
+    <t>DENG, CHERI X; FU, JIANPING  (contact);</t>
+  </si>
+  <si>
+    <t>10272357</t>
+  </si>
+  <si>
+    <t>HAYDEN GEPHART, MELANIE ;</t>
+  </si>
+  <si>
+    <t>10271736</t>
+  </si>
+  <si>
+    <t>TAVAZOIE, SOHAIL F.;</t>
+  </si>
+  <si>
+    <t>10270593</t>
+  </si>
+  <si>
+    <t>DEUSTACHIO, PETER G (contact); MUNGALL, CHRISTOPHER J; SMITH, CYNTHIA LOUISE; THOMAS, PAUL D.;</t>
+  </si>
+  <si>
+    <t>10270036</t>
+  </si>
+  <si>
+    <t>WU, CATHERINE JU-YING;</t>
+  </si>
+  <si>
+    <t>10269797</t>
+  </si>
+  <si>
+    <t>DAVIS</t>
+  </si>
+  <si>
+    <t>MIGLIORETTI, DIANA L;</t>
+  </si>
+  <si>
+    <t>10267051</t>
+  </si>
+  <si>
+    <t>DUONG, VU H.;</t>
+  </si>
+  <si>
+    <t>10266277</t>
+  </si>
+  <si>
+    <t>GILKEY, MELISSA B;</t>
+  </si>
+  <si>
+    <t>10256080</t>
+  </si>
+  <si>
+    <t>METZGER, CORINNE ;</t>
+  </si>
+  <si>
+    <t>10210586</t>
+  </si>
+  <si>
+    <t>PISCATAWAY</t>
+  </si>
+  <si>
+    <t>XIAO, SHUO ;</t>
+  </si>
+  <si>
+    <t>10127885</t>
+  </si>
+  <si>
+    <t>YOON, JIN HO;</t>
+  </si>
+  <si>
+    <t>10102061</t>
+  </si>
+  <si>
+    <t>SHARP, ANDREW JAMES;</t>
+  </si>
+  <si>
+    <t>10101736</t>
+  </si>
+  <si>
+    <t>WHITNEY, DANIEL ;</t>
+  </si>
+  <si>
+    <t>10070242</t>
+  </si>
+  <si>
+    <t>WEST KINGSTON</t>
+  </si>
+  <si>
+    <t>DESPLAN, CLAUDE ;</t>
+  </si>
+  <si>
+    <t>Virtual Reality for Panic Disorder With Agoraphobia</t>
+  </si>
+  <si>
+    <t>Complete</t>
+  </si>
+  <si>
+    <t>Gustavsberg primary care center, Gustavsberg, Stockholm, Sweden|Karolinska Institutet, Stockholm, Sweden</t>
+  </si>
+  <si>
+    <t>Title</t>
+  </si>
+  <si>
+    <t>Status</t>
+  </si>
+  <si>
+    <t>Locations</t>
+  </si>
+  <si>
+    <t>Thought Field Therapy and Cognitive Therapy for Agoraphobia</t>
+  </si>
+  <si>
+    <t>Sorlandet Hospital, Arendal, Norway</t>
+  </si>
+  <si>
+    <t>Study of Virtual Reality Therapy and Cognitive Behavior Therapy in Panic Disorder With Agoraphobia</t>
+  </si>
+  <si>
+    <t>Unknown statu</t>
+  </si>
+  <si>
+    <t>HÃ´pital Pierre Wertheimer, Bron, France</t>
+  </si>
+  <si>
+    <t>Physical Activity and Cognitive Behavioural Therapy in Panic Disorder and Agoraphobia</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>Mechanisms of Treatment Change in Panic Disorder and Agoraphobia</t>
+  </si>
+  <si>
+    <t>Southern Methodist University, Department of Psychology, Dallas, Texas, United States</t>
+  </si>
+  <si>
+    <t>Longterm Outcome of Inpatient Cognitive and Behavioral Therapies for Agoraphobia</t>
+  </si>
+  <si>
+    <t>Modum Bad, Vikersund, Norway</t>
+  </si>
+  <si>
+    <t>Efficacy of Hypnotherapy for Agoraphobia</t>
+  </si>
+  <si>
+    <t>Prof. Dr. A. Batra/ Dr. Kristina Fuhr, University Department for Psychiatry and Psychotherapie, Tuebingen, Germany</t>
+  </si>
+  <si>
+    <t>Effectiveness of Intensive Cognitive Behavioral Therapy in Treating Adolescent Panic Disorder and Agoraphobia</t>
+  </si>
+  <si>
+    <t>Boston University, Boston, Massachusetts, United States</t>
+  </si>
+  <si>
+    <t>Cognitive Behavior Therapy vs Exposure in Vivo in the Treatment of Panic Disorder With Agoraphobia</t>
+  </si>
+  <si>
+    <t>Recruitin</t>
+  </si>
+  <si>
+    <t>Zentrum fÃ¼r Psychotherapie, Bochum, NRW, Germany</t>
+  </si>
+  <si>
+    <t>Augmentation of Psychotherapy With D-Cycloserine in Agoraphobia</t>
+  </si>
+  <si>
+    <t>Department of Psychiatry and Psychotherapy, CharitÃ© Campus Mitte - UniversitÃ¤tsmedizin Berlin, Berlin, Germany</t>
   </si>
 </sst>
 </file>
@@ -1048,4 +1482,714 @@
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <dimension ref="B1:D52"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.0"/>
+  <sheetData>
+    <row r="1"/>
+    <row r="2">
+      <c r="B2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="B3" t="s">
+        <v>141</v>
+      </c>
+      <c r="C3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D3" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="B4" t="s">
+        <v>143</v>
+      </c>
+      <c r="C4" t="s">
+        <v>144</v>
+      </c>
+      <c r="D4" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="B5" t="s">
+        <v>146</v>
+      </c>
+      <c r="C5" t="s">
+        <v>147</v>
+      </c>
+      <c r="D5" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="B6" t="s">
+        <v>149</v>
+      </c>
+      <c r="C6" t="s">
+        <v>150</v>
+      </c>
+      <c r="D6" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="B7" t="s">
+        <v>152</v>
+      </c>
+      <c r="C7" t="s">
+        <v>153</v>
+      </c>
+      <c r="D7" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="B8" t="s">
+        <v>155</v>
+      </c>
+      <c r="C8" t="s">
+        <v>13</v>
+      </c>
+      <c r="D8" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="B9" t="s">
+        <v>157</v>
+      </c>
+      <c r="C9" t="s">
+        <v>58</v>
+      </c>
+      <c r="D9" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="B10" t="s">
+        <v>159</v>
+      </c>
+      <c r="C10" t="s">
+        <v>28</v>
+      </c>
+      <c r="D10" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="B11" t="s">
+        <v>161</v>
+      </c>
+      <c r="C11" t="s">
+        <v>162</v>
+      </c>
+      <c r="D11" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="B12" t="s">
+        <v>164</v>
+      </c>
+      <c r="C12" t="s">
+        <v>58</v>
+      </c>
+      <c r="D12" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="B13" t="s">
+        <v>166</v>
+      </c>
+      <c r="C13" t="s">
+        <v>37</v>
+      </c>
+      <c r="D13" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="B14" t="s">
+        <v>168</v>
+      </c>
+      <c r="C14" t="s">
+        <v>129</v>
+      </c>
+      <c r="D14" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="B15" t="s">
+        <v>170</v>
+      </c>
+      <c r="C15" t="s">
+        <v>107</v>
+      </c>
+      <c r="D15" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="B16" t="s">
+        <v>172</v>
+      </c>
+      <c r="C16" t="s">
+        <v>13</v>
+      </c>
+      <c r="D16" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="B17" t="s">
+        <v>174</v>
+      </c>
+      <c r="C17" t="s">
+        <v>175</v>
+      </c>
+      <c r="D17" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="B18" t="s">
+        <v>177</v>
+      </c>
+      <c r="C18" t="s">
+        <v>4</v>
+      </c>
+      <c r="D18" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="B19" t="s">
+        <v>179</v>
+      </c>
+      <c r="C19" t="s">
+        <v>58</v>
+      </c>
+      <c r="D19" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="B20" t="s">
+        <v>181</v>
+      </c>
+      <c r="C20" t="s">
+        <v>28</v>
+      </c>
+      <c r="D20" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="B21" t="s">
+        <v>183</v>
+      </c>
+      <c r="C21" t="s">
+        <v>184</v>
+      </c>
+      <c r="D21" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="B22" t="s">
+        <v>186</v>
+      </c>
+      <c r="C22" t="s">
+        <v>13</v>
+      </c>
+      <c r="D22" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="B23" t="s">
+        <v>188</v>
+      </c>
+      <c r="C23" t="s">
+        <v>175</v>
+      </c>
+      <c r="D23" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="B24" t="s">
+        <v>190</v>
+      </c>
+      <c r="C24" t="s">
+        <v>175</v>
+      </c>
+      <c r="D24" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="B25" t="s">
+        <v>192</v>
+      </c>
+      <c r="C25" t="s">
+        <v>107</v>
+      </c>
+      <c r="D25" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="B26" t="s">
+        <v>194</v>
+      </c>
+      <c r="C26" t="s">
+        <v>10</v>
+      </c>
+      <c r="D26" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="B27" t="s">
+        <v>196</v>
+      </c>
+      <c r="C27" t="s">
+        <v>4</v>
+      </c>
+      <c r="D27" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="B28" t="s">
+        <v>198</v>
+      </c>
+      <c r="C28" t="s">
+        <v>88</v>
+      </c>
+      <c r="D28" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="B29" t="s">
+        <v>200</v>
+      </c>
+      <c r="C29" t="s">
+        <v>201</v>
+      </c>
+      <c r="D29" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="B30" t="s">
+        <v>203</v>
+      </c>
+      <c r="C30" t="s">
+        <v>204</v>
+      </c>
+      <c r="D30" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="B31" t="s">
+        <v>206</v>
+      </c>
+      <c r="C31" t="s">
+        <v>13</v>
+      </c>
+      <c r="D31" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="B32" t="s">
+        <v>208</v>
+      </c>
+      <c r="C32" t="s">
+        <v>209</v>
+      </c>
+      <c r="D32" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="B33" t="s">
+        <v>211</v>
+      </c>
+      <c r="C33" t="s">
+        <v>212</v>
+      </c>
+      <c r="D33" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="B34" t="s">
+        <v>214</v>
+      </c>
+      <c r="C34" t="s">
+        <v>215</v>
+      </c>
+      <c r="D34" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="B35" t="s">
+        <v>217</v>
+      </c>
+      <c r="C35" t="s">
+        <v>218</v>
+      </c>
+      <c r="D35" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="B36" t="s">
+        <v>220</v>
+      </c>
+      <c r="C36" t="s">
+        <v>218</v>
+      </c>
+      <c r="D36" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="B37" t="s">
+        <v>222</v>
+      </c>
+      <c r="C37" t="s">
+        <v>223</v>
+      </c>
+      <c r="D37" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="B38" t="s">
+        <v>225</v>
+      </c>
+      <c r="C38" t="s">
+        <v>28</v>
+      </c>
+      <c r="D38" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="B39" t="s">
+        <v>227</v>
+      </c>
+      <c r="C39" t="s">
+        <v>110</v>
+      </c>
+      <c r="D39" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="B40" t="s">
+        <v>229</v>
+      </c>
+      <c r="C40" t="s">
+        <v>72</v>
+      </c>
+      <c r="D40" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="B41" t="s">
+        <v>231</v>
+      </c>
+      <c r="C41" t="s">
+        <v>4</v>
+      </c>
+      <c r="D41" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="B42" t="s">
+        <v>233</v>
+      </c>
+      <c r="C42" t="s">
+        <v>4</v>
+      </c>
+      <c r="D42" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="B43" t="s">
+        <v>235</v>
+      </c>
+      <c r="C43" t="s">
+        <v>13</v>
+      </c>
+      <c r="D43" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="B44" t="s">
+        <v>237</v>
+      </c>
+      <c r="C44" t="s">
+        <v>238</v>
+      </c>
+      <c r="D44" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="B45" t="s">
+        <v>240</v>
+      </c>
+      <c r="C45" t="s">
+        <v>28</v>
+      </c>
+      <c r="D45" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="B46" t="s">
+        <v>242</v>
+      </c>
+      <c r="C46" t="s">
+        <v>58</v>
+      </c>
+      <c r="D46" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="B47" t="s">
+        <v>244</v>
+      </c>
+      <c r="C47" t="s">
+        <v>50</v>
+      </c>
+      <c r="D47" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="B48" t="s">
+        <v>246</v>
+      </c>
+      <c r="C48" t="s">
+        <v>247</v>
+      </c>
+      <c r="D48" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="B49" t="s">
+        <v>249</v>
+      </c>
+      <c r="C49" t="s">
+        <v>107</v>
+      </c>
+      <c r="D49" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="B50" t="s">
+        <v>251</v>
+      </c>
+      <c r="C50" t="s">
+        <v>4</v>
+      </c>
+      <c r="D50" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="B51" t="s">
+        <v>253</v>
+      </c>
+      <c r="C51" t="s">
+        <v>110</v>
+      </c>
+      <c r="D51" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="B52" t="s">
+        <v>255</v>
+      </c>
+      <c r="C52" t="s">
+        <v>256</v>
+      </c>
+      <c r="D52" t="s">
+        <v>257</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <dimension ref="B1:D12"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.0"/>
+  <sheetData>
+    <row r="1"/>
+    <row r="2">
+      <c r="B2" t="s">
+        <v>258</v>
+      </c>
+      <c r="C2" t="s">
+        <v>259</v>
+      </c>
+      <c r="D2" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="B3" t="s">
+        <v>261</v>
+      </c>
+      <c r="C3" t="s">
+        <v>262</v>
+      </c>
+      <c r="D3" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="B4" t="s">
+        <v>264</v>
+      </c>
+      <c r="C4" t="s">
+        <v>259</v>
+      </c>
+      <c r="D4" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="B5" t="s">
+        <v>266</v>
+      </c>
+      <c r="C5" t="s">
+        <v>267</v>
+      </c>
+      <c r="D5" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="B6" t="s">
+        <v>269</v>
+      </c>
+      <c r="C6" t="s">
+        <v>259</v>
+      </c>
+      <c r="D6" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="B7" t="s">
+        <v>271</v>
+      </c>
+      <c r="C7" t="s">
+        <v>259</v>
+      </c>
+      <c r="D7" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="B8" t="s">
+        <v>273</v>
+      </c>
+      <c r="C8" t="s">
+        <v>259</v>
+      </c>
+      <c r="D8" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="B9" t="s">
+        <v>275</v>
+      </c>
+      <c r="C9" t="s">
+        <v>259</v>
+      </c>
+      <c r="D9" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="B10" t="s">
+        <v>277</v>
+      </c>
+      <c r="C10" t="s">
+        <v>259</v>
+      </c>
+      <c r="D10" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="B11" t="s">
+        <v>279</v>
+      </c>
+      <c r="C11" t="s">
+        <v>280</v>
+      </c>
+      <c r="D11" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="B12" t="s">
+        <v>282</v>
+      </c>
+      <c r="C12" t="s">
+        <v>259</v>
+      </c>
+      <c r="D12" t="s">
+        <v>283</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+</worksheet>
 </file>
</xml_diff>